<commit_message>
update python-openstackclient deps xlsx file
</commit_message>
<xml_diff>
--- a/25.1.Epoxy/i8.OS.Other.Projects/i8.23.python-openstackclient.deps.xlsx
+++ b/25.1.Epoxy/i8.OS.Other.Projects/i8.23.python-openstackclient.deps.xlsx
@@ -971,7 +971,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1011,13 +1011,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00A933"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF2A6099"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1083,7 +1076,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1136,14 +1129,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1152,7 +1137,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1193,7 +1178,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1409,10 +1394,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD483"/>
+  <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A403" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A417" activeCellId="0" sqref="417:417"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1773,27 +1758,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="13" t="s">
+    <row r="21" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="14" t="n">
+      <c r="E21" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
@@ -1823,7 +1808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>43</v>
@@ -1892,7 +1877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1987,7 +1972,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2082,7 +2067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2099,7 +2084,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -2226,7 +2211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2243,7 +2228,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -2312,7 +2297,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2468,35 +2453,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="13" t="s">
+    <row r="53" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="13" t="s">
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K53" s="13" t="s">
+      <c r="K53" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>43</v>
@@ -2570,27 +2555,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="13" t="s">
+    <row r="59" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="14" t="n">
+      <c r="E59" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F59" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="7" t="s">
@@ -2676,7 +2661,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>43</v>
@@ -2806,7 +2791,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
@@ -2955,7 +2940,7 @@
       <c r="M76" s="8" t="n">
         <v>2.4</v>
       </c>
-      <c r="N76" s="16" t="s">
+      <c r="N76" s="14" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3070,7 +3055,7 @@
       <c r="M82" s="8" t="n">
         <v>2.4</v>
       </c>
-      <c r="N82" s="16" t="s">
+      <c r="N82" s="14" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3107,7 +3092,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
@@ -3407,35 +3392,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="13" t="s">
+    <row r="102" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D102" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E102" s="14" t="s">
+      <c r="E102" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F102" s="14" t="s">
+      <c r="F102" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G102" s="14" t="s">
+      <c r="G102" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H102" s="14"/>
-      <c r="I102" s="14"/>
-      <c r="J102" s="13" t="s">
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K102" s="13" t="s">
+      <c r="K102" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1"/>
       <c r="B103" s="1" t="s">
         <v>43</v>
@@ -3534,7 +3519,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
@@ -3642,35 +3627,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="13" t="s">
+    <row r="115" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D115" s="13" t="s">
+      <c r="D115" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E115" s="14" t="s">
+      <c r="E115" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F115" s="14" t="s">
+      <c r="F115" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G115" s="14" t="s">
+      <c r="G115" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="13" t="s">
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K115" s="13" t="s">
+      <c r="K115" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="116" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="B116" s="1" t="s">
         <v>43</v>
@@ -3706,36 +3691,36 @@
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
     </row>
-    <row r="118" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="13" t="s">
+    <row r="118" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D118" s="13" t="s">
+      <c r="D118" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="E118" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F118" s="14" t="s">
+      <c r="F118" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G118" s="14" t="s">
+      <c r="G118" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H118" s="14" t="s">
+      <c r="H118" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I118" s="14"/>
-      <c r="J118" s="13" t="s">
+      <c r="I118" s="9"/>
+      <c r="J118" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="K118" s="13" t="s">
+      <c r="K118" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3744,31 +3729,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="13" t="s">
+    <row r="121" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C121" s="13" t="s">
+      <c r="C121" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D121" s="13" t="s">
+      <c r="D121" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E121" s="14" t="s">
+      <c r="E121" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F121" s="14" t="s">
+      <c r="F121" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G121" s="14" t="s">
+      <c r="G121" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="13" t="s">
+      <c r="H121" s="9"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K121" s="13" t="s">
+      <c r="K121" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3891,27 +3876,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="13" t="s">
+    <row r="137" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C137" s="13" t="s">
+      <c r="C137" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D137" s="13" t="s">
+      <c r="D137" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E137" s="14" t="n">
+      <c r="E137" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F137" s="14" t="s">
+      <c r="F137" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G137" s="14" t="s">
+      <c r="G137" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H137" s="14"/>
-      <c r="I137" s="14"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
     </row>
     <row r="138" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="7" t="s">
@@ -4025,31 +4010,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="142" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="13" t="s">
+    <row r="142" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B142" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C142" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D142" s="13" t="s">
+      <c r="D142" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E142" s="14" t="s">
+      <c r="E142" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F142" s="14" t="s">
+      <c r="F142" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G142" s="14" t="s">
+      <c r="G142" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H142" s="14"/>
-      <c r="I142" s="14"/>
-      <c r="J142" s="13" t="s">
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K142" s="13" t="s">
+      <c r="K142" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4081,7 +4066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="144" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="7"/>
       <c r="B144" s="7" t="s">
         <v>92</v>
@@ -4114,91 +4099,91 @@
       <c r="N144" s="7"/>
       <c r="O144" s="7"/>
     </row>
-    <row r="145" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="13" t="s">
+    <row r="145" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C145" s="13" t="s">
+      <c r="C145" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D145" s="13" t="s">
+      <c r="D145" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E145" s="14" t="s">
+      <c r="E145" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F145" s="14" t="s">
+      <c r="F145" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G145" s="14" t="s">
+      <c r="G145" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H145" s="14"/>
-      <c r="I145" s="14"/>
-      <c r="J145" s="13" t="s">
+      <c r="H145" s="9"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K145" s="13" t="s">
+      <c r="K145" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="146" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="13" t="s">
+    <row r="146" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B146" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C146" s="13" t="s">
+      <c r="C146" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D146" s="13" t="s">
+      <c r="D146" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E146" s="14" t="s">
+      <c r="E146" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F146" s="14" t="s">
+      <c r="F146" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G146" s="14" t="s">
+      <c r="G146" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H146" s="14"/>
-      <c r="I146" s="14"/>
-      <c r="J146" s="13" t="s">
+      <c r="H146" s="9"/>
+      <c r="I146" s="9"/>
+      <c r="J146" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K146" s="13" t="s">
+      <c r="K146" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="147" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="13" t="s">
+    <row r="147" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B147" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C147" s="13" t="s">
+      <c r="C147" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D147" s="13" t="s">
+      <c r="D147" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E147" s="14" t="s">
+      <c r="E147" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F147" s="14" t="s">
+      <c r="F147" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G147" s="14" t="s">
+      <c r="G147" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H147" s="14"/>
-      <c r="I147" s="14"/>
-      <c r="J147" s="13" t="s">
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K147" s="13" t="s">
+      <c r="K147" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="148" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
       <c r="B148" s="1" t="s">
         <v>43</v>
@@ -4267,7 +4252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4284,7 +4269,7 @@
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
     </row>
-    <row r="152" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
         <v>20</v>
       </c>
@@ -4303,7 +4288,7 @@
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
     </row>
-    <row r="153" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4322,7 +4307,7 @@
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
     </row>
-    <row r="154" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4341,7 +4326,7 @@
       <c r="N154" s="1"/>
       <c r="O154" s="1"/>
     </row>
-    <row r="155" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4360,7 +4345,7 @@
       <c r="N155" s="1"/>
       <c r="O155" s="1"/>
     </row>
-    <row r="156" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4405,7 +4390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="158" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4533,7 +4518,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="164" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4631,7 +4616,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="168" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4676,7 +4661,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4726,63 +4711,63 @@
         <v>42</v>
       </c>
     </row>
-    <row r="173" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="13" t="s">
+    <row r="173" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C173" s="13" t="s">
+      <c r="C173" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D173" s="13" t="s">
+      <c r="D173" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E173" s="14" t="s">
+      <c r="E173" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F173" s="14" t="s">
+      <c r="F173" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G173" s="14" t="s">
+      <c r="G173" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H173" s="14"/>
-      <c r="I173" s="14"/>
-      <c r="J173" s="13" t="s">
+      <c r="H173" s="9"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K173" s="13" t="s">
+      <c r="K173" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="174" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="13" t="s">
+    <row r="174" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B174" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C174" s="13" t="s">
+      <c r="C174" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D174" s="13" t="s">
+      <c r="D174" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E174" s="14" t="s">
+      <c r="E174" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F174" s="14" t="s">
+      <c r="F174" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G174" s="14" t="s">
+      <c r="G174" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H174" s="14"/>
-      <c r="I174" s="14"/>
-      <c r="J174" s="13" t="s">
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K174" s="13" t="s">
+      <c r="K174" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="175" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
       <c r="B175" s="1" t="s">
         <v>43</v>
@@ -4818,7 +4803,7 @@
       <c r="N176" s="10"/>
       <c r="O176" s="10"/>
     </row>
-    <row r="177" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4835,7 +4820,7 @@
       <c r="N177" s="1"/>
       <c r="O177" s="1"/>
     </row>
-    <row r="178" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4852,7 +4837,7 @@
       <c r="N178" s="1"/>
       <c r="O178" s="1"/>
     </row>
-    <row r="179" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4869,7 +4854,7 @@
       <c r="N179" s="1"/>
       <c r="O179" s="1"/>
     </row>
-    <row r="180" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4948,7 +4933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="184" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4965,7 +4950,7 @@
       <c r="N184" s="1"/>
       <c r="O184" s="1"/>
     </row>
-    <row r="185" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
         <v>20</v>
       </c>
@@ -4984,7 +4969,7 @@
       <c r="N185" s="1"/>
       <c r="O185" s="1"/>
     </row>
-    <row r="186" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -5003,7 +4988,7 @@
       <c r="N186" s="1"/>
       <c r="O186" s="1"/>
     </row>
-    <row r="187" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -5022,7 +5007,7 @@
       <c r="N187" s="1"/>
       <c r="O187" s="1"/>
     </row>
-    <row r="188" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -5041,7 +5026,7 @@
       <c r="N188" s="1"/>
       <c r="O188" s="1"/>
     </row>
-    <row r="189" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -5083,7 +5068,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="191" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -5105,49 +5090,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="193" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D193" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E193" s="9" t="s">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="E193" s="9" t="n">
+        <v>45840</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G193" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H193" s="9"/>
       <c r="I193" s="9"/>
-      <c r="J193" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K193" s="7" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="194" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="7" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="D194" s="7" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="E194" s="9" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="F194" s="9" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G194" s="9" t="s">
         <v>10</v>
@@ -5155,27 +5134,27 @@
       <c r="H194" s="9"/>
       <c r="I194" s="9"/>
       <c r="J194" s="7" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="K194" s="7" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
     </row>
     <row r="195" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="7" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D195" s="7" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="E195" s="9" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F195" s="9" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="G195" s="9" t="s">
         <v>10</v>
@@ -5183,147 +5162,153 @@
       <c r="H195" s="9"/>
       <c r="I195" s="9"/>
       <c r="J195" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K195" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="196" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E196" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F196" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G196" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H196" s="9"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K195" s="7" t="s">
+      <c r="K196" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="196" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="13" t="s">
+    <row r="197" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B197" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C196" s="13" t="s">
+      <c r="C197" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D196" s="13" t="s">
+      <c r="D197" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E196" s="14" t="s">
+      <c r="E197" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F196" s="14" t="s">
+      <c r="F197" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G196" s="14" t="s">
+      <c r="G197" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H196" s="14"/>
-      <c r="I196" s="14"/>
-      <c r="J196" s="13" t="s">
+      <c r="H197" s="9"/>
+      <c r="I197" s="9"/>
+      <c r="J197" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K196" s="13" t="s">
+      <c r="K197" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="197" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="13" t="s">
+    <row r="198" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C197" s="13" t="s">
+      <c r="C198" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D197" s="13" t="s">
+      <c r="D198" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E197" s="14" t="s">
+      <c r="E198" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F197" s="14" t="s">
+      <c r="F198" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G197" s="14" t="s">
+      <c r="G198" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H197" s="14"/>
-      <c r="I197" s="14"/>
-      <c r="J197" s="13" t="s">
+      <c r="H198" s="9"/>
+      <c r="I198" s="9"/>
+      <c r="J198" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K197" s="13" t="s">
+      <c r="K198" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="198" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="13" t="s">
+    <row r="199" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B199" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C198" s="13" t="s">
+      <c r="C199" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D198" s="13" t="s">
+      <c r="D199" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E198" s="14" t="s">
+      <c r="E199" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F198" s="14" t="s">
+      <c r="F199" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G198" s="14" t="s">
+      <c r="G199" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H198" s="14"/>
-      <c r="I198" s="14"/>
-      <c r="J198" s="13" t="s">
+      <c r="H199" s="9"/>
+      <c r="I199" s="9"/>
+      <c r="J199" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K198" s="13" t="s">
+      <c r="K199" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="199" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="13" t="s">
+    <row r="200" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B200" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C199" s="13" t="s">
+      <c r="C200" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D199" s="13" t="s">
+      <c r="D200" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E199" s="14" t="s">
+      <c r="E200" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F199" s="14" t="s">
+      <c r="F200" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G199" s="14" t="s">
+      <c r="G200" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H199" s="14"/>
-      <c r="I199" s="14"/>
-      <c r="J199" s="13" t="s">
+      <c r="H200" s="9"/>
+      <c r="I200" s="9"/>
+      <c r="J200" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K199" s="13" t="s">
+      <c r="K200" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="200" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C200" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D200" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E200" s="14" t="n">
-        <v>45840</v>
-      </c>
-      <c r="F200" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G200" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H200" s="14"/>
-      <c r="I200" s="14"/>
-    </row>
-    <row r="201" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1"/>
       <c r="B201" s="1" t="s">
         <v>43</v>
@@ -5392,7 +5377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="204" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -5409,7 +5394,7 @@
       <c r="N204" s="1"/>
       <c r="O204" s="1"/>
     </row>
-    <row r="205" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
         <v>20</v>
       </c>
@@ -5568,7 +5553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="211" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -5590,57 +5575,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="13" t="s">
+    <row r="213" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B213" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C213" s="13" t="s">
+      <c r="C213" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D213" s="13" t="s">
+      <c r="D213" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E213" s="14" t="n">
+      <c r="E213" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F213" s="14" t="s">
+      <c r="F213" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G213" s="14" t="s">
+      <c r="G213" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H213" s="14"/>
-      <c r="I213" s="14"/>
+      <c r="H213" s="9"/>
+      <c r="I213" s="9"/>
     </row>
-    <row r="214" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="13" t="s">
+    <row r="214" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B214" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C214" s="13" t="s">
+      <c r="C214" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D214" s="13" t="s">
+      <c r="D214" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E214" s="14" t="s">
+      <c r="E214" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F214" s="14" t="s">
+      <c r="F214" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G214" s="14" t="s">
+      <c r="G214" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H214" s="14"/>
-      <c r="I214" s="14"/>
-      <c r="J214" s="13" t="s">
+      <c r="H214" s="9"/>
+      <c r="I214" s="9"/>
+      <c r="J214" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K214" s="13" t="s">
+      <c r="K214" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="215" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1"/>
       <c r="B215" s="1" t="s">
         <v>43</v>
@@ -5709,7 +5694,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="218" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -5726,7 +5711,7 @@
       <c r="N218" s="1"/>
       <c r="O218" s="1"/>
     </row>
-    <row r="219" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
         <v>20</v>
       </c>
@@ -5745,7 +5730,7 @@
       <c r="N219" s="1"/>
       <c r="O219" s="1"/>
     </row>
-    <row r="220" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -5764,7 +5749,7 @@
       <c r="N220" s="1"/>
       <c r="O220" s="1"/>
     </row>
-    <row r="221" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -5783,7 +5768,7 @@
       <c r="N221" s="1"/>
       <c r="O221" s="1"/>
     </row>
-    <row r="222" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -5802,7 +5787,7 @@
       <c r="N222" s="1"/>
       <c r="O222" s="1"/>
     </row>
-    <row r="223" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -5819,7 +5804,7 @@
       <c r="N223" s="1"/>
       <c r="O223" s="1"/>
     </row>
-    <row r="224" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -5838,7 +5823,7 @@
       <c r="N224" s="1"/>
       <c r="O224" s="1"/>
     </row>
-    <row r="225" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -5855,7 +5840,7 @@
       <c r="N225" s="1"/>
       <c r="O225" s="1"/>
     </row>
-    <row r="226" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -5874,7 +5859,7 @@
       <c r="N226" s="1"/>
       <c r="O226" s="1"/>
     </row>
-    <row r="227" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -5893,7 +5878,7 @@
       <c r="N227" s="1"/>
       <c r="O227" s="1"/>
     </row>
-    <row r="228" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -5912,7 +5897,7 @@
       <c r="N228" s="1"/>
       <c r="O228" s="1"/>
     </row>
-    <row r="229" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -5931,7 +5916,7 @@
       <c r="N229" s="1"/>
       <c r="O229" s="1"/>
     </row>
-    <row r="230" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -5950,7 +5935,7 @@
       <c r="N230" s="1"/>
       <c r="O230" s="1"/>
     </row>
-    <row r="231" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -5969,7 +5954,7 @@
       <c r="N231" s="1"/>
       <c r="O231" s="1"/>
     </row>
-    <row r="232" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -6154,7 +6139,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="239" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -6204,91 +6189,91 @@
         <v>42</v>
       </c>
     </row>
-    <row r="242" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="13" t="s">
+    <row r="242" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B242" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C242" s="13" t="s">
+      <c r="C242" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D242" s="13" t="s">
+      <c r="D242" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E242" s="14" t="s">
+      <c r="E242" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F242" s="14" t="s">
+      <c r="F242" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G242" s="14" t="s">
+      <c r="G242" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H242" s="14"/>
-      <c r="I242" s="14"/>
-      <c r="J242" s="13" t="s">
+      <c r="H242" s="9"/>
+      <c r="I242" s="9"/>
+      <c r="J242" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K242" s="13" t="s">
+      <c r="K242" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="243" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="13" t="s">
+    <row r="243" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B243" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C243" s="13" t="s">
+      <c r="C243" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D243" s="13" t="s">
+      <c r="D243" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E243" s="14" t="s">
+      <c r="E243" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F243" s="14" t="s">
+      <c r="F243" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G243" s="14" t="s">
+      <c r="G243" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H243" s="14"/>
-      <c r="I243" s="14"/>
-      <c r="J243" s="13" t="s">
+      <c r="H243" s="9"/>
+      <c r="I243" s="9"/>
+      <c r="J243" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K243" s="13" t="s">
+      <c r="K243" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="244" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="13" t="s">
+    <row r="244" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B244" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C244" s="13" t="s">
+      <c r="C244" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D244" s="13" t="s">
+      <c r="D244" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E244" s="14" t="s">
+      <c r="E244" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F244" s="14" t="s">
+      <c r="F244" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G244" s="14" t="s">
+      <c r="G244" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H244" s="14"/>
-      <c r="I244" s="14"/>
-      <c r="J244" s="13" t="s">
+      <c r="H244" s="9"/>
+      <c r="I244" s="9"/>
+      <c r="J244" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K244" s="13" t="s">
+      <c r="K244" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="245" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1"/>
       <c r="B245" s="1" t="s">
         <v>43</v>
@@ -6324,7 +6309,7 @@
       <c r="N246" s="10"/>
       <c r="O246" s="10"/>
     </row>
-    <row r="247" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -6341,7 +6326,7 @@
       <c r="N247" s="1"/>
       <c r="O247" s="1"/>
     </row>
-    <row r="248" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -6455,7 +6440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="269" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
@@ -6472,7 +6457,7 @@
       <c r="N269" s="1"/>
       <c r="O269" s="1"/>
     </row>
-    <row r="270" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
         <v>20</v>
       </c>
@@ -6491,7 +6476,7 @@
       <c r="N270" s="1"/>
       <c r="O270" s="1"/>
     </row>
-    <row r="271" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
@@ -6510,7 +6495,7 @@
       <c r="N271" s="1"/>
       <c r="O271" s="1"/>
     </row>
-    <row r="272" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
@@ -6529,7 +6514,7 @@
       <c r="N272" s="1"/>
       <c r="O272" s="1"/>
     </row>
-    <row r="273" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
@@ -6548,7 +6533,7 @@
       <c r="N273" s="1"/>
       <c r="O273" s="1"/>
     </row>
-    <row r="274" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
@@ -6617,7 +6602,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="277" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
@@ -6639,27 +6624,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="279" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B279" s="13" t="s">
+    <row r="279" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B279" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C279" s="13" t="s">
+      <c r="C279" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D279" s="13" t="s">
+      <c r="D279" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E279" s="14" t="n">
+      <c r="E279" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F279" s="14" t="s">
+      <c r="F279" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G279" s="14" t="s">
+      <c r="G279" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H279" s="14"/>
-      <c r="I279" s="14"/>
+      <c r="H279" s="9"/>
+      <c r="I279" s="9"/>
     </row>
     <row r="280" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="7" t="s">
@@ -6689,119 +6674,119 @@
         <v>42</v>
       </c>
     </row>
-    <row r="281" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="13" t="s">
+    <row r="281" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B281" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C281" s="13" t="s">
+      <c r="C281" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D281" s="13" t="s">
+      <c r="D281" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E281" s="14" t="s">
+      <c r="E281" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F281" s="14" t="s">
+      <c r="F281" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G281" s="14" t="s">
+      <c r="G281" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H281" s="14"/>
-      <c r="I281" s="14"/>
-      <c r="J281" s="13" t="s">
+      <c r="H281" s="9"/>
+      <c r="I281" s="9"/>
+      <c r="J281" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K281" s="13" t="s">
+      <c r="K281" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="282" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B282" s="13" t="s">
+    <row r="282" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B282" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C282" s="13" t="s">
+      <c r="C282" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D282" s="13" t="s">
+      <c r="D282" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E282" s="14" t="s">
+      <c r="E282" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F282" s="14" t="s">
+      <c r="F282" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G282" s="14" t="s">
+      <c r="G282" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H282" s="14"/>
-      <c r="I282" s="14"/>
-      <c r="J282" s="13" t="s">
+      <c r="H282" s="9"/>
+      <c r="I282" s="9"/>
+      <c r="J282" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K282" s="13" t="s">
+      <c r="K282" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="283" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="13" t="s">
+    <row r="283" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B283" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C283" s="13" t="s">
+      <c r="C283" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D283" s="13" t="s">
+      <c r="D283" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E283" s="14" t="s">
+      <c r="E283" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F283" s="14" t="s">
+      <c r="F283" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G283" s="14" t="s">
+      <c r="G283" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H283" s="14"/>
-      <c r="I283" s="14"/>
-      <c r="J283" s="13" t="s">
+      <c r="H283" s="9"/>
+      <c r="I283" s="9"/>
+      <c r="J283" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K283" s="13" t="s">
+      <c r="K283" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="284" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="13" t="s">
+    <row r="284" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B284" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C284" s="13" t="s">
+      <c r="C284" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D284" s="13" t="s">
+      <c r="D284" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E284" s="14" t="s">
+      <c r="E284" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F284" s="14" t="s">
+      <c r="F284" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G284" s="14" t="s">
+      <c r="G284" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H284" s="14"/>
-      <c r="I284" s="14"/>
-      <c r="J284" s="13" t="s">
+      <c r="H284" s="9"/>
+      <c r="I284" s="9"/>
+      <c r="J284" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K284" s="13" t="s">
+      <c r="K284" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="285" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1"/>
       <c r="B285" s="1" t="s">
         <v>43</v>
@@ -6837,36 +6822,36 @@
       <c r="N286" s="10"/>
       <c r="O286" s="10"/>
     </row>
-    <row r="287" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="13" t="s">
+    <row r="287" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B287" s="13" t="s">
+      <c r="B287" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C287" s="13" t="s">
+      <c r="C287" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D287" s="13" t="s">
+      <c r="D287" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E287" s="14" t="s">
+      <c r="E287" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F287" s="14" t="s">
+      <c r="F287" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G287" s="14" t="s">
+      <c r="G287" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H287" s="14" t="s">
+      <c r="H287" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I287" s="14"/>
-      <c r="J287" s="13" t="s">
+      <c r="I287" s="9"/>
+      <c r="J287" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K287" s="13" t="s">
+      <c r="K287" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7004,31 +6989,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="298" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B298" s="13" t="s">
+    <row r="298" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C298" s="13" t="s">
+      <c r="C298" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D298" s="13" t="s">
+      <c r="D298" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E298" s="14" t="s">
+      <c r="E298" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F298" s="14" t="s">
+      <c r="F298" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G298" s="14" t="s">
+      <c r="G298" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H298" s="14"/>
-      <c r="I298" s="14"/>
-      <c r="J298" s="13" t="s">
+      <c r="H298" s="9"/>
+      <c r="I298" s="9"/>
+      <c r="J298" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="K298" s="13" t="s">
+      <c r="K298" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7089,34 +7074,34 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A302" s="13" t="s">
+    <row r="302" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A302" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B302" s="13" t="s">
+      <c r="B302" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C302" s="13" t="s">
+      <c r="C302" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D302" s="13" t="s">
+      <c r="D302" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E302" s="14" t="s">
+      <c r="E302" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F302" s="14" t="s">
+      <c r="F302" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G302" s="14" t="s">
+      <c r="G302" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H302" s="14"/>
-      <c r="I302" s="14"/>
-      <c r="J302" s="13" t="s">
+      <c r="H302" s="9"/>
+      <c r="I302" s="9"/>
+      <c r="J302" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K302" s="13" t="s">
+      <c r="K302" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7137,7 +7122,7 @@
       <c r="N303" s="10"/>
       <c r="O303" s="10"/>
     </row>
-    <row r="304" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
@@ -7154,7 +7139,7 @@
       <c r="N304" s="1"/>
       <c r="O304" s="1"/>
     </row>
-    <row r="305" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
@@ -7171,7 +7156,7 @@
       <c r="N305" s="1"/>
       <c r="O305" s="1"/>
     </row>
-    <row r="306" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
@@ -7238,7 +7223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="309" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
@@ -7255,7 +7240,7 @@
       <c r="N309" s="1"/>
       <c r="O309" s="1"/>
     </row>
-    <row r="310" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
         <v>20</v>
       </c>
@@ -7274,7 +7259,7 @@
       <c r="N310" s="1"/>
       <c r="O310" s="1"/>
     </row>
-    <row r="311" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
@@ -7293,7 +7278,7 @@
       <c r="N311" s="1"/>
       <c r="O311" s="1"/>
     </row>
-    <row r="312" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
@@ -7312,7 +7297,7 @@
       <c r="N312" s="1"/>
       <c r="O312" s="1"/>
     </row>
-    <row r="313" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
@@ -7331,7 +7316,7 @@
       <c r="N313" s="1"/>
       <c r="O313" s="1"/>
     </row>
-    <row r="314" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
@@ -7348,7 +7333,7 @@
       <c r="N314" s="1"/>
       <c r="O314" s="1"/>
     </row>
-    <row r="315" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
@@ -7367,7 +7352,7 @@
       <c r="N315" s="1"/>
       <c r="O315" s="1"/>
     </row>
-    <row r="316" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
@@ -7386,7 +7371,7 @@
       <c r="N316" s="1"/>
       <c r="O316" s="1"/>
     </row>
-    <row r="317" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
@@ -7405,7 +7390,7 @@
       <c r="N317" s="1"/>
       <c r="O317" s="1"/>
     </row>
-    <row r="318" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
@@ -7424,7 +7409,7 @@
       <c r="N318" s="1"/>
       <c r="O318" s="1"/>
     </row>
-    <row r="319" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
@@ -7588,7 +7573,7 @@
       <c r="C325" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D325" s="18" t="s">
+      <c r="D325" s="16" t="s">
         <v>257</v>
       </c>
       <c r="E325" s="9" t="s">
@@ -7616,7 +7601,7 @@
       <c r="C326" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D326" s="18" t="s">
+      <c r="D326" s="16" t="s">
         <v>260</v>
       </c>
       <c r="E326" s="9" t="s">
@@ -7727,7 +7712,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="330" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1"/>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -7749,119 +7734,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="332" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="13" t="s">
+    <row r="332" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B332" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C332" s="13" t="s">
+      <c r="C332" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D332" s="13" t="s">
+      <c r="D332" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E332" s="14" t="s">
+      <c r="E332" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F332" s="14" t="s">
+      <c r="F332" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G332" s="14" t="s">
+      <c r="G332" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H332" s="14"/>
-      <c r="I332" s="14"/>
-      <c r="J332" s="13" t="s">
+      <c r="H332" s="9"/>
+      <c r="I332" s="9"/>
+      <c r="J332" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K332" s="13" t="s">
+      <c r="K332" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="333" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B333" s="13" t="s">
+    <row r="333" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B333" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C333" s="13" t="s">
+      <c r="C333" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D333" s="13" t="s">
+      <c r="D333" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E333" s="14" t="s">
+      <c r="E333" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F333" s="14" t="s">
+      <c r="F333" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G333" s="14" t="s">
+      <c r="G333" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H333" s="14"/>
-      <c r="I333" s="14"/>
-      <c r="J333" s="13" t="s">
+      <c r="H333" s="9"/>
+      <c r="I333" s="9"/>
+      <c r="J333" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K333" s="13" t="s">
+      <c r="K333" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="334" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B334" s="13" t="s">
+    <row r="334" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B334" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C334" s="13" t="s">
+      <c r="C334" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D334" s="13" t="s">
+      <c r="D334" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E334" s="14" t="s">
+      <c r="E334" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F334" s="14" t="s">
+      <c r="F334" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G334" s="14" t="s">
+      <c r="G334" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H334" s="14"/>
-      <c r="I334" s="14"/>
-      <c r="J334" s="13" t="s">
+      <c r="H334" s="9"/>
+      <c r="I334" s="9"/>
+      <c r="J334" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K334" s="13" t="s">
+      <c r="K334" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="335" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B335" s="13" t="s">
+    <row r="335" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B335" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C335" s="13" t="s">
+      <c r="C335" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D335" s="13" t="s">
+      <c r="D335" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E335" s="14" t="s">
+      <c r="E335" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F335" s="14" t="s">
+      <c r="F335" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G335" s="14" t="s">
+      <c r="G335" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H335" s="14"/>
-      <c r="I335" s="14"/>
-      <c r="J335" s="13" t="s">
+      <c r="H335" s="9"/>
+      <c r="I335" s="9"/>
+      <c r="J335" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K335" s="13" t="s">
+      <c r="K335" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="336" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1"/>
       <c r="B336" s="1" t="s">
         <v>43</v>
@@ -7897,40 +7882,40 @@
       <c r="N337" s="10"/>
       <c r="O337" s="10"/>
     </row>
-    <row r="338" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="13" t="s">
+    <row r="338" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B338" s="13" t="s">
+      <c r="B338" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C338" s="13" t="s">
+      <c r="C338" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D338" s="13" t="s">
+      <c r="D338" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E338" s="14" t="s">
+      <c r="E338" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F338" s="14" t="s">
+      <c r="F338" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G338" s="14" t="s">
+      <c r="G338" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H338" s="14" t="s">
+      <c r="H338" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I338" s="14"/>
-      <c r="J338" s="13" t="s">
+      <c r="I338" s="9"/>
+      <c r="J338" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K338" s="13" t="s">
+      <c r="K338" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="339" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1"/>
       <c r="B339" s="1"/>
       <c r="C339" s="1"/>
@@ -7947,7 +7932,7 @@
       <c r="N339" s="1"/>
       <c r="O339" s="1"/>
     </row>
-    <row r="340" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
         <v>20</v>
       </c>
@@ -7966,7 +7951,7 @@
       <c r="N340" s="1"/>
       <c r="O340" s="1"/>
     </row>
-    <row r="341" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
       <c r="C341" s="1"/>
@@ -7985,7 +7970,7 @@
       <c r="N341" s="1"/>
       <c r="O341" s="1"/>
     </row>
-    <row r="342" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
@@ -8004,7 +7989,7 @@
       <c r="N342" s="1"/>
       <c r="O342" s="1"/>
     </row>
-    <row r="343" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1"/>
       <c r="B343" s="1"/>
       <c r="C343" s="1"/>
@@ -8023,7 +8008,7 @@
       <c r="N343" s="1"/>
       <c r="O343" s="1"/>
     </row>
-    <row r="344" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -8040,7 +8025,7 @@
       <c r="N344" s="1"/>
       <c r="O344" s="1"/>
     </row>
-    <row r="345" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1"/>
       <c r="B345" s="1"/>
       <c r="C345" s="1"/>
@@ -8059,7 +8044,7 @@
       <c r="N345" s="1"/>
       <c r="O345" s="1"/>
     </row>
-    <row r="346" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1"/>
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
@@ -8078,7 +8063,7 @@
       <c r="N346" s="1"/>
       <c r="O346" s="1"/>
     </row>
-    <row r="347" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1"/>
@@ -8097,7 +8082,7 @@
       <c r="N347" s="1"/>
       <c r="O347" s="1"/>
     </row>
-    <row r="348" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1"/>
       <c r="B348" s="1"/>
       <c r="C348" s="1"/>
@@ -8116,7 +8101,7 @@
       <c r="N348" s="1"/>
       <c r="O348" s="1"/>
     </row>
-    <row r="349" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
       <c r="C349" s="1"/>
@@ -8133,31 +8118,31 @@
       <c r="N349" s="1"/>
       <c r="O349" s="1"/>
     </row>
-    <row r="350" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B350" s="13" t="s">
+    <row r="350" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B350" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C350" s="13" t="s">
+      <c r="C350" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="D350" s="13" t="s">
+      <c r="D350" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="E350" s="14" t="s">
+      <c r="E350" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F350" s="14" t="s">
+      <c r="F350" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="G350" s="14" t="s">
+      <c r="G350" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H350" s="14"/>
-      <c r="I350" s="14"/>
-      <c r="J350" s="13" t="s">
+      <c r="H350" s="9"/>
+      <c r="I350" s="9"/>
+      <c r="J350" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="K350" s="13" t="s">
+      <c r="K350" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -8189,7 +8174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="352" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="1"/>
       <c r="B352" s="7" t="s">
         <v>157</v>
@@ -8197,7 +8182,7 @@
       <c r="C352" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D352" s="18" t="s">
+      <c r="D352" s="16" t="s">
         <v>260</v>
       </c>
       <c r="E352" s="9" t="s">
@@ -8222,7 +8207,7 @@
       <c r="N352" s="1"/>
       <c r="O352" s="1"/>
     </row>
-    <row r="353" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="1"/>
       <c r="B353" s="1"/>
       <c r="C353" s="1"/>
@@ -8239,34 +8224,34 @@
       <c r="N353" s="1"/>
       <c r="O353" s="1"/>
     </row>
-    <row r="354" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A354" s="13" t="s">
+    <row r="354" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A354" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B354" s="13" t="s">
+      <c r="B354" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C354" s="13" t="s">
+      <c r="C354" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D354" s="13" t="s">
+      <c r="D354" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E354" s="14" t="s">
+      <c r="E354" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F354" s="14" t="s">
+      <c r="F354" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G354" s="14" t="s">
+      <c r="G354" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H354" s="14"/>
-      <c r="I354" s="14"/>
-      <c r="J354" s="13" t="s">
+      <c r="H354" s="9"/>
+      <c r="I354" s="9"/>
+      <c r="J354" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K354" s="13" t="s">
+      <c r="K354" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -8287,7 +8272,7 @@
       <c r="N355" s="10"/>
       <c r="O355" s="10"/>
     </row>
-    <row r="356" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="1"/>
       <c r="B356" s="1"/>
       <c r="C356" s="1"/>
@@ -8304,7 +8289,7 @@
       <c r="N356" s="1"/>
       <c r="O356" s="1"/>
     </row>
-    <row r="357" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="1"/>
       <c r="B357" s="1"/>
       <c r="C357" s="1"/>
@@ -8321,7 +8306,7 @@
       <c r="N357" s="1"/>
       <c r="O357" s="1"/>
     </row>
-    <row r="358" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="1"/>
       <c r="B358" s="1"/>
       <c r="C358" s="1"/>
@@ -8338,7 +8323,7 @@
       <c r="N358" s="1"/>
       <c r="O358" s="1"/>
     </row>
-    <row r="359" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="1"/>
       <c r="B359" s="1"/>
       <c r="C359" s="1"/>
@@ -8511,7 +8496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="370" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1"/>
       <c r="B370" s="1" t="s">
         <v>43</v>
@@ -8547,7 +8532,7 @@
       <c r="N371" s="10"/>
       <c r="O371" s="10"/>
     </row>
-    <row r="372" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1"/>
       <c r="B372" s="1"/>
       <c r="C372" s="1"/>
@@ -8629,7 +8614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="376" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1"/>
       <c r="B376" s="1"/>
       <c r="C376" s="1"/>
@@ -8646,7 +8631,7 @@
       <c r="N376" s="1"/>
       <c r="O376" s="1"/>
     </row>
-    <row r="377" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="s">
         <v>20</v>
       </c>
@@ -9063,7 +9048,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="392" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="392" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="1"/>
       <c r="B392" s="1"/>
       <c r="C392" s="1"/>
@@ -9085,57 +9070,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="394" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B394" s="13" t="s">
+    <row r="394" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B394" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C394" s="13" t="s">
+      <c r="C394" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D394" s="13" t="s">
+      <c r="D394" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E394" s="14" t="n">
+      <c r="E394" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F394" s="14" t="s">
+      <c r="F394" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G394" s="14" t="s">
+      <c r="G394" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H394" s="14"/>
-      <c r="I394" s="14"/>
+      <c r="H394" s="9"/>
+      <c r="I394" s="9"/>
     </row>
-    <row r="395" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B395" s="13" t="s">
+    <row r="395" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B395" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C395" s="13" t="s">
+      <c r="C395" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D395" s="13" t="s">
+      <c r="D395" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E395" s="14" t="s">
+      <c r="E395" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F395" s="14" t="s">
+      <c r="F395" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G395" s="14" t="s">
+      <c r="G395" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H395" s="14"/>
-      <c r="I395" s="14"/>
-      <c r="J395" s="13" t="s">
+      <c r="H395" s="9"/>
+      <c r="I395" s="9"/>
+      <c r="J395" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K395" s="13" t="s">
+      <c r="K395" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="396" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1"/>
       <c r="B396" s="1" t="s">
         <v>43</v>
@@ -9171,40 +9156,40 @@
       <c r="N397" s="10"/>
       <c r="O397" s="10"/>
     </row>
-    <row r="398" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A398" s="13" t="s">
+    <row r="398" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A398" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B398" s="13" t="s">
+      <c r="B398" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C398" s="13" t="s">
+      <c r="C398" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D398" s="13" t="s">
+      <c r="D398" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E398" s="14" t="s">
+      <c r="E398" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F398" s="14" t="s">
+      <c r="F398" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G398" s="14" t="s">
+      <c r="G398" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H398" s="14" t="s">
+      <c r="H398" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I398" s="14"/>
-      <c r="J398" s="13" t="s">
+      <c r="I398" s="9"/>
+      <c r="J398" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K398" s="13" t="s">
+      <c r="K398" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="399" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="399" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1"/>
       <c r="B399" s="1"/>
       <c r="C399" s="1"/>
@@ -9221,7 +9206,7 @@
       <c r="N399" s="1"/>
       <c r="O399" s="1"/>
     </row>
-    <row r="400" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
         <v>20</v>
       </c>
@@ -9240,7 +9225,7 @@
       <c r="N400" s="1"/>
       <c r="O400" s="1"/>
     </row>
-    <row r="401" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1"/>
       <c r="B401" s="1"/>
       <c r="C401" s="1"/>
@@ -9259,7 +9244,7 @@
       <c r="N401" s="1"/>
       <c r="O401" s="1"/>
     </row>
-    <row r="402" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1"/>
       <c r="B402" s="1"/>
       <c r="C402" s="1"/>
@@ -9278,7 +9263,7 @@
       <c r="N402" s="1"/>
       <c r="O402" s="1"/>
     </row>
-    <row r="403" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1"/>
       <c r="B403" s="1"/>
       <c r="C403" s="1"/>
@@ -9297,7 +9282,7 @@
       <c r="N403" s="1"/>
       <c r="O403" s="1"/>
     </row>
-    <row r="404" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1"/>
       <c r="B404" s="1"/>
       <c r="C404" s="1"/>
@@ -9342,7 +9327,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="406" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1"/>
       <c r="B406" s="1"/>
       <c r="C406" s="1"/>
@@ -9555,7 +9540,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="414" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1"/>
       <c r="B414" s="1"/>
       <c r="C414" s="1"/>
@@ -9577,57 +9562,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="416" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="13" t="s">
+    <row r="416" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B416" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C416" s="13" t="s">
+      <c r="C416" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D416" s="13" t="s">
+      <c r="D416" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E416" s="14" t="n">
+      <c r="E416" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F416" s="14" t="s">
+      <c r="F416" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G416" s="14" t="s">
+      <c r="G416" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H416" s="14"/>
-      <c r="I416" s="14"/>
+      <c r="H416" s="9"/>
+      <c r="I416" s="9"/>
     </row>
-    <row r="417" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B417" s="13" t="s">
+    <row r="417" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B417" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C417" s="13" t="s">
+      <c r="C417" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D417" s="13" t="s">
+      <c r="D417" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E417" s="14" t="s">
+      <c r="E417" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F417" s="14" t="s">
+      <c r="F417" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G417" s="14" t="s">
+      <c r="G417" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H417" s="14"/>
-      <c r="I417" s="14"/>
-      <c r="J417" s="13" t="s">
+      <c r="H417" s="9"/>
+      <c r="I417" s="9"/>
+      <c r="J417" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K417" s="13" t="s">
+      <c r="K417" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="418" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1"/>
       <c r="B418" s="1" t="s">
         <v>43</v>
@@ -9663,7 +9648,7 @@
       <c r="N419" s="10"/>
       <c r="O419" s="10"/>
     </row>
-    <row r="420" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1"/>
       <c r="B420" s="1"/>
       <c r="C420" s="1"/>
@@ -9680,7 +9665,7 @@
       <c r="N420" s="1"/>
       <c r="O420" s="1"/>
     </row>
-    <row r="421" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1"/>
       <c r="B421" s="1"/>
       <c r="C421" s="1"/>
@@ -26083,40 +26068,40 @@
       <c r="XFC422" s="0"/>
       <c r="XFD422" s="0"/>
     </row>
-    <row r="423" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A423" s="13" t="s">
+    <row r="423" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A423" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B423" s="13" t="s">
+      <c r="B423" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C423" s="13" t="s">
+      <c r="C423" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D423" s="13" t="s">
+      <c r="D423" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E423" s="14" t="s">
+      <c r="E423" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F423" s="14" t="s">
+      <c r="F423" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G423" s="14" t="s">
+      <c r="G423" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H423" s="14" t="s">
+      <c r="H423" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I423" s="14"/>
-      <c r="J423" s="13" t="s">
+      <c r="I423" s="9"/>
+      <c r="J423" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K423" s="13" t="s">
+      <c r="K423" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="424" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1"/>
       <c r="B424" s="1"/>
       <c r="C424" s="1"/>
@@ -26133,7 +26118,7 @@
       <c r="N424" s="1"/>
       <c r="O424" s="1"/>
     </row>
-    <row r="425" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="s">
         <v>20</v>
       </c>
@@ -26152,7 +26137,7 @@
       <c r="N425" s="1"/>
       <c r="O425" s="1"/>
     </row>
-    <row r="426" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1"/>
       <c r="B426" s="1"/>
       <c r="C426" s="1"/>
@@ -26171,7 +26156,7 @@
       <c r="N426" s="1"/>
       <c r="O426" s="1"/>
     </row>
-    <row r="427" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1"/>
       <c r="B427" s="1"/>
       <c r="C427" s="1"/>
@@ -26190,7 +26175,7 @@
       <c r="N427" s="1"/>
       <c r="O427" s="1"/>
     </row>
-    <row r="428" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1"/>
       <c r="B428" s="1"/>
       <c r="C428" s="1"/>
@@ -26209,7 +26194,7 @@
       <c r="N428" s="1"/>
       <c r="O428" s="1"/>
     </row>
-    <row r="429" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1"/>
       <c r="B429" s="1"/>
       <c r="C429" s="1"/>
@@ -26422,7 +26407,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="437" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1"/>
       <c r="B437" s="1"/>
       <c r="C437" s="1"/>
@@ -26439,30 +26424,30 @@
       <c r="N437" s="1"/>
       <c r="O437" s="1"/>
     </row>
-    <row r="438" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="13" t="s">
+    <row r="438" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B438" s="13" t="s">
+      <c r="B438" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C438" s="13" t="s">
+      <c r="C438" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D438" s="13" t="s">
+      <c r="D438" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E438" s="14" t="n">
+      <c r="E438" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F438" s="14" t="s">
+      <c r="F438" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G438" s="14" t="s">
+      <c r="G438" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H438" s="14"/>
-      <c r="I438" s="14"/>
+      <c r="H438" s="9"/>
+      <c r="I438" s="9"/>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="10"/>
@@ -42850,40 +42835,40 @@
       <c r="XFC439" s="0"/>
       <c r="XFD439" s="0"/>
     </row>
-    <row r="440" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A440" s="13" t="s">
+    <row r="440" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A440" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B440" s="13" t="s">
+      <c r="B440" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C440" s="13" t="s">
+      <c r="C440" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D440" s="13" t="s">
+      <c r="D440" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E440" s="14" t="s">
+      <c r="E440" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F440" s="14" t="s">
+      <c r="F440" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G440" s="14" t="s">
+      <c r="G440" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H440" s="14" t="s">
+      <c r="H440" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I440" s="14"/>
-      <c r="J440" s="13" t="s">
+      <c r="I440" s="9"/>
+      <c r="J440" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K440" s="13" t="s">
+      <c r="K440" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="441" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1"/>
       <c r="B441" s="1"/>
       <c r="C441" s="1"/>
@@ -42900,7 +42885,7 @@
       <c r="N441" s="1"/>
       <c r="O441" s="1"/>
     </row>
-    <row r="442" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
         <v>20</v>
       </c>
@@ -42919,7 +42904,7 @@
       <c r="N442" s="1"/>
       <c r="O442" s="1"/>
     </row>
-    <row r="443" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="443" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1"/>
       <c r="B443" s="1"/>
       <c r="C443" s="1"/>
@@ -42937,29 +42922,29 @@
       <c r="M443" s="1"/>
       <c r="N443" s="1"/>
       <c r="O443" s="1"/>
-      <c r="R443" s="15" t="s">
+      <c r="R443" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="S443" s="15" t="s">
+      <c r="S443" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="T443" s="15" t="s">
+      <c r="T443" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="U443" s="15" t="s">
+      <c r="U443" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="V443" s="15" t="s">
+      <c r="V443" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="W443" s="15" t="s">
+      <c r="W443" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="X443" s="15" t="s">
+      <c r="X443" s="13" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="444" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1"/>
       <c r="B444" s="1"/>
       <c r="C444" s="1"/>
@@ -42977,35 +42962,35 @@
       <c r="M444" s="1"/>
       <c r="N444" s="1"/>
       <c r="O444" s="1"/>
-      <c r="R444" s="15" t="s">
+      <c r="R444" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="S444" s="15" t="s">
+      <c r="S444" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="T444" s="15" t="s">
+      <c r="T444" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="U444" s="15" t="s">
+      <c r="U444" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="V444" s="15" t="s">
+      <c r="V444" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="W444" s="15" t="s">
+      <c r="W444" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="X444" s="15" t="s">
+      <c r="X444" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="Y444" s="15" t="s">
+      <c r="Y444" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="Z444" s="15" t="s">
+      <c r="Z444" s="13" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="445" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1"/>
       <c r="B445" s="1"/>
       <c r="C445" s="1"/>
@@ -43023,22 +43008,22 @@
       <c r="M445" s="1"/>
       <c r="N445" s="1"/>
       <c r="O445" s="1"/>
-      <c r="R445" s="15" t="s">
+      <c r="R445" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="S445" s="15" t="s">
+      <c r="S445" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="T445" s="15" t="s">
+      <c r="T445" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="U445" s="15" t="s">
+      <c r="U445" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="V445" s="15" t="s">
+      <c r="V445" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W445" s="15" t="s">
+      <c r="W445" s="13" t="s">
         <v>308</v>
       </c>
     </row>
@@ -43070,7 +43055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="447" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="1"/>
       <c r="B447" s="1"/>
       <c r="C447" s="1"/>
@@ -43143,31 +43128,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="450" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B450" s="13" t="s">
+    <row r="450" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B450" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C450" s="13" t="s">
+      <c r="C450" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D450" s="13" t="s">
+      <c r="D450" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E450" s="14" t="s">
+      <c r="E450" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F450" s="14" t="s">
+      <c r="F450" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G450" s="14" t="s">
+      <c r="G450" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H450" s="14"/>
-      <c r="I450" s="14"/>
-      <c r="J450" s="13" t="s">
+      <c r="H450" s="9"/>
+      <c r="I450" s="9"/>
+      <c r="J450" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K450" s="13" t="s">
+      <c r="K450" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -43199,31 +43184,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="452" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B452" s="13" t="s">
+    <row r="452" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B452" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C452" s="13" t="s">
+      <c r="C452" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D452" s="13" t="s">
+      <c r="D452" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E452" s="14" t="s">
+      <c r="E452" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F452" s="14" t="s">
+      <c r="F452" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G452" s="14" t="s">
+      <c r="G452" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H452" s="14"/>
-      <c r="I452" s="14"/>
-      <c r="J452" s="13" t="s">
+      <c r="H452" s="9"/>
+      <c r="I452" s="9"/>
+      <c r="J452" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="K452" s="13" t="s">
+      <c r="K452" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -43318,7 +43303,7 @@
       <c r="C456" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D456" s="18" t="s">
+      <c r="D456" s="16" t="s">
         <v>257</v>
       </c>
       <c r="E456" s="9" t="s">
@@ -43339,7 +43324,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="457" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="1"/>
       <c r="B457" s="1"/>
       <c r="C457" s="1"/>
@@ -43356,30 +43341,30 @@
       <c r="N457" s="1"/>
       <c r="O457" s="1"/>
     </row>
-    <row r="458" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="13" t="s">
+    <row r="458" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B458" s="13" t="s">
+      <c r="B458" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C458" s="13" t="s">
+      <c r="C458" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D458" s="13" t="s">
+      <c r="D458" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E458" s="14" t="n">
+      <c r="E458" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F458" s="14" t="s">
+      <c r="F458" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G458" s="14" t="s">
+      <c r="G458" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H458" s="14"/>
-      <c r="I458" s="14"/>
+      <c r="H458" s="9"/>
+      <c r="I458" s="9"/>
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="10"/>
@@ -43398,7 +43383,7 @@
       <c r="N459" s="10"/>
       <c r="O459" s="10"/>
     </row>
-    <row r="460" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="1"/>
       <c r="B460" s="1"/>
       <c r="C460" s="1"/>
@@ -43415,7 +43400,7 @@
       <c r="N460" s="1"/>
       <c r="O460" s="1"/>
     </row>
-    <row r="461" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1"/>
       <c r="B461" s="1"/>
       <c r="C461" s="1"/>
@@ -43432,7 +43417,7 @@
       <c r="N461" s="1"/>
       <c r="O461" s="1"/>
     </row>
-    <row r="462" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="462" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1"/>
       <c r="B462" s="1"/>
       <c r="C462" s="1"/>
@@ -43478,32 +43463,32 @@
       <c r="N464" s="10"/>
       <c r="O464" s="10"/>
     </row>
-    <row r="465" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="13" t="s">
+    <row r="465" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B465" s="13" t="s">
+      <c r="B465" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C465" s="13" t="s">
+      <c r="C465" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D465" s="13" t="s">
+      <c r="D465" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E465" s="14" t="n">
+      <c r="E465" s="9" t="n">
         <v>45840</v>
       </c>
-      <c r="F465" s="14" t="s">
+      <c r="F465" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G465" s="14" t="s">
+      <c r="G465" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H465" s="14" t="s">
+      <c r="H465" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I465" s="14"/>
+      <c r="I465" s="9"/>
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
@@ -43671,31 +43656,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="478" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B478" s="13" t="s">
+    <row r="478" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B478" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C478" s="13" t="s">
+      <c r="C478" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D478" s="13" t="s">
+      <c r="D478" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E478" s="14" t="s">
+      <c r="E478" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F478" s="14" t="s">
+      <c r="F478" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G478" s="14" t="s">
+      <c r="G478" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H478" s="14"/>
-      <c r="I478" s="14"/>
-      <c r="J478" s="13" t="s">
+      <c r="H478" s="9"/>
+      <c r="I478" s="9"/>
+      <c r="J478" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K478" s="13" t="s">
+      <c r="K478" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -43727,59 +43712,59 @@
         <v>42</v>
       </c>
     </row>
-    <row r="480" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B480" s="13" t="s">
+    <row r="480" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B480" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C480" s="13" t="s">
+      <c r="C480" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D480" s="13" t="s">
+      <c r="D480" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E480" s="14" t="s">
+      <c r="E480" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F480" s="14" t="s">
+      <c r="F480" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G480" s="14" t="s">
+      <c r="G480" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H480" s="14"/>
-      <c r="I480" s="14"/>
-      <c r="J480" s="13" t="s">
+      <c r="H480" s="9"/>
+      <c r="I480" s="9"/>
+      <c r="J480" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K480" s="13" t="s">
+      <c r="K480" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="481" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B481" s="13" t="s">
+    <row r="481" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B481" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C481" s="13" t="s">
+      <c r="C481" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D481" s="13" t="s">
+      <c r="D481" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E481" s="14" t="s">
+      <c r="E481" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F481" s="14" t="s">
+      <c r="F481" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G481" s="14" t="s">
+      <c r="G481" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H481" s="14"/>
-      <c r="I481" s="14"/>
-      <c r="J481" s="13" t="s">
+      <c r="H481" s="9"/>
+      <c r="I481" s="9"/>
+      <c r="J481" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K481" s="13" t="s">
+      <c r="K481" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -43839,6 +43824,7 @@
         <v>42</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>